<commit_message>
Barclays data and facility labels
</commit_message>
<xml_diff>
--- a/app/assets/downloads/Barclays-status-report-June-2023.xlsx
+++ b/app/assets/downloads/Barclays-status-report-June-2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Documents/Prototypes/ukef/prototypekit-stb-bank/app/assets/downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4670E66E-02AC-AD4D-B1AB-38FB57D74192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDB55BD-4B2B-7040-97D6-D5B3DCBDC047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-200" yWindow="-30260" windowWidth="41460" windowHeight="20200" xr2:uid="{6BDF98CE-C6B7-004B-B507-299FF645EC01}"/>
+    <workbookView xWindow="2060" yWindow="-29180" windowWidth="41460" windowHeight="20200" xr2:uid="{6BDF98CE-C6B7-004B-B507-299FF645EC01}"/>
   </bookViews>
   <sheets>
     <sheet name="Download" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="60">
   <si>
     <t>UKEF facility ID</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Product type</t>
   </si>
   <si>
-    <t>Bank primary reference</t>
-  </si>
-  <si>
     <t>Bank secondary reference</t>
   </si>
   <si>
@@ -154,6 +151,72 @@
   </si>
   <si>
     <t>6p1.41</t>
+  </si>
+  <si>
+    <t>Able Robotics Ltd</t>
+  </si>
+  <si>
+    <t>Britannia Energy GEF</t>
+  </si>
+  <si>
+    <t>FutureTech Innovators GEF</t>
+  </si>
+  <si>
+    <t>NexGen Robotics GEF</t>
+  </si>
+  <si>
+    <t>Union Manufacturing GEF</t>
+  </si>
+  <si>
+    <t>Marine Equipment GEF</t>
+  </si>
+  <si>
+    <t>Innovate Solutions GEF</t>
+  </si>
+  <si>
+    <t>LuminaTech Gef</t>
+  </si>
+  <si>
+    <t>Able Robotics GEF</t>
+  </si>
+  <si>
+    <t>Energy Solutions GEF</t>
+  </si>
+  <si>
+    <t>Automation Solutions GEF</t>
+  </si>
+  <si>
+    <t>British Engineering Solutions GEF</t>
+  </si>
+  <si>
+    <t>Meridian Manufacturing GEF</t>
+  </si>
+  <si>
+    <t>AirTech GEF</t>
+  </si>
+  <si>
+    <t>ADB Aeronautics GEF</t>
+  </si>
+  <si>
+    <t>Mighty Manufacturing GEF</t>
+  </si>
+  <si>
+    <t>DLS GEF</t>
+  </si>
+  <si>
+    <t>Precision Engineering GEF</t>
+  </si>
+  <si>
+    <t>PPS Ltd GEF</t>
+  </si>
+  <si>
+    <t>SynopSolutions Ltd GEF</t>
+  </si>
+  <si>
+    <t>Cryo Construction GEF</t>
+  </si>
+  <si>
+    <t>Bank reference</t>
   </si>
 </sst>
 </file>
@@ -240,9 +303,7 @@
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,7 +630,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="22.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="22" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="37" style="1" customWidth="1"/>
@@ -586,10 +647,10 @@
   <sheetData>
     <row r="3" spans="2:13" s="5" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>0</v>
@@ -623,8 +684,8 @@
       </c>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B4" s="10">
-        <v>3001175147</v>
+      <c r="B4" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4">
@@ -650,8 +711,8 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="10">
-        <v>3001184276</v>
+      <c r="B5" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4">
@@ -677,8 +738,8 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10">
-        <v>3001193729</v>
+      <c r="B6" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="4">
@@ -704,8 +765,8 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="10">
-        <v>3001201721</v>
+      <c r="B7" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4">
@@ -731,8 +792,8 @@
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="10">
-        <v>3001210542</v>
+      <c r="B8" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4">
@@ -758,8 +819,8 @@
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="10">
-        <v>3001224759</v>
+      <c r="B9" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4">
@@ -785,8 +846,8 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="10">
-        <v>3001248940</v>
+      <c r="B10" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="4">
@@ -812,15 +873,15 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="10">
-        <v>3001258036</v>
+      <c r="B11" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4">
         <v>20001987</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>26</v>
@@ -839,8 +900,8 @@
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="10">
-        <v>3001269305</v>
+      <c r="B12" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="4">
@@ -866,8 +927,8 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="10">
-        <v>3001274983</v>
+      <c r="B13" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="4">
@@ -893,8 +954,8 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="10">
-        <v>3001289791</v>
+      <c r="B14" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="4">
@@ -920,8 +981,8 @@
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="10">
-        <v>3001291749</v>
+      <c r="B15" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="4">
@@ -947,8 +1008,8 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="10">
-        <v>3001294859</v>
+      <c r="B16" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="4">
@@ -974,8 +1035,8 @@
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="10">
-        <v>3001300128</v>
+      <c r="B17" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="4">
@@ -1001,8 +1062,8 @@
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="10">
-        <v>3001300635</v>
+      <c r="B18" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="4">
@@ -1028,8 +1089,8 @@
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="10">
-        <v>3001301749</v>
+      <c r="B19" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="4">
@@ -1055,8 +1116,8 @@
       <c r="L19" s="9"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="10">
-        <v>3001308367</v>
+      <c r="B20" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="4">
@@ -1082,8 +1143,8 @@
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="10">
-        <v>3001313461</v>
+      <c r="B21" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4">
@@ -1109,8 +1170,8 @@
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="10">
-        <v>3001326729</v>
+      <c r="B22" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4">
@@ -1136,8 +1197,8 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="10">
-        <v>3001378304</v>
+      <c r="B23" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4">
@@ -1176,7 +1237,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="37" style="1" customWidth="1"/>
@@ -1193,10 +1254,10 @@
   <sheetData>
     <row r="3" spans="2:13" s="5" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>0</v>
@@ -1230,8 +1291,8 @@
       </c>
     </row>
     <row r="4" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="10">
-        <v>3001175147</v>
+      <c r="B4" s="10" t="s">
+        <v>39</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4">
@@ -1253,7 +1314,7 @@
         <v>600000</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" s="9">
         <v>367.23</v>
@@ -1263,8 +1324,8 @@
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="10">
-        <v>3001184276</v>
+      <c r="B5" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4">
@@ -1296,8 +1357,8 @@
       </c>
     </row>
     <row r="6" spans="2:13" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="10">
-        <v>3001193729</v>
+      <c r="B6" s="10" t="s">
+        <v>41</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="4">
@@ -1327,8 +1388,8 @@
       </c>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="10">
-        <v>3001201721</v>
+      <c r="B7" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="4">
@@ -1360,8 +1421,8 @@
       </c>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="10">
-        <v>3001210542</v>
+      <c r="B8" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="4">
@@ -1393,8 +1454,8 @@
       </c>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="10">
-        <v>3001224759</v>
+      <c r="B9" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="4">
@@ -1426,8 +1487,8 @@
       </c>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="10">
-        <v>3001248940</v>
+      <c r="B10" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="4">
@@ -1459,15 +1520,15 @@
       </c>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="10">
-        <v>3001258036</v>
+      <c r="B11" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="4">
         <v>20001987</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>26</v>
@@ -1492,8 +1553,8 @@
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="10">
-        <v>3001269305</v>
+      <c r="B12" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="4">
@@ -1525,8 +1586,8 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="10">
-        <v>3001274983</v>
+      <c r="B13" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="4">
@@ -1558,8 +1619,8 @@
       </c>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="10">
-        <v>3001289791</v>
+      <c r="B14" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="4">
@@ -1591,8 +1652,8 @@
       </c>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="10">
-        <v>3001291749</v>
+      <c r="B15" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="4">
@@ -1624,8 +1685,8 @@
       </c>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="10">
-        <v>3001294859</v>
+      <c r="B16" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="4">
@@ -1657,8 +1718,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B17" s="10">
-        <v>3001300128</v>
+      <c r="B17" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="4">
@@ -1686,12 +1747,12 @@
         <v>601.41</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B18" s="10">
-        <v>3001300635</v>
+      <c r="B18" s="10" t="s">
+        <v>53</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="4">
@@ -1723,8 +1784,8 @@
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="10">
-        <v>3001301749</v>
+      <c r="B19" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="4">
@@ -1756,8 +1817,8 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="10">
-        <v>3001308367</v>
+      <c r="B20" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="4">
@@ -1789,8 +1850,8 @@
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="10">
-        <v>3001313461</v>
+      <c r="B21" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="4">
@@ -1822,8 +1883,8 @@
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="10">
-        <v>3001326729</v>
+      <c r="B22" s="10" t="s">
+        <v>57</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="4">
@@ -1855,8 +1916,8 @@
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B23" s="10">
-        <v>3001378304</v>
+      <c r="B23" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="4">

</xml_diff>